<commit_message>
Renforcement de l'import + génération d'une install
</commit_message>
<xml_diff>
--- a/src/test/resources/fr/remiguitreau/aroeven/barcode/xls/equipments_ok.xlsx
+++ b/src/test/resources/fr/remiguitreau/aroeven/barcode/xls/equipments_ok.xlsx
@@ -56,6 +56,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -77,11 +78,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -224,13 +227,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -298,7 +301,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D4" type="list">

</xml_diff>

<commit_message>
On organise les codes barres par modèles.
</commit_message>
<xml_diff>
--- a/src/test/resources/fr/remiguitreau/aroeven/barcode/xls/equipments_ok.xlsx
+++ b/src/test/resources/fr/remiguitreau/aroeven/barcode/xls/equipments_ok.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="182" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="72" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Marque</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Oui</t>
+  </si>
+  <si>
+    <t>Head</t>
   </si>
   <si>
     <t>Helmet</t>
@@ -230,10 +233,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -291,19 +294,33 @@
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="B5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D4" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D5" type="list">
       <formula1>"Oui,Non"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>